<commit_message>
print diff and overlap stats
</commit_message>
<xml_diff>
--- a/artifacts/classification.xlsx
+++ b/artifacts/classification.xlsx
@@ -222,270 +222,273 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="121">
+  <si>
+    <t>BCoordLang</t>
+  </si>
+  <si>
+    <t>BCOoL</t>
+  </si>
+  <si>
+    <t>Ptolemy</t>
+  </si>
+  <si>
+    <t>Wright (ADL)</t>
+  </si>
+  <si>
+    <t>MontiArc (ADL)</t>
+  </si>
+  <si>
+    <t>CommUnity (ADL)</t>
+  </si>
+  <si>
+    <t>Metropolis</t>
+  </si>
+  <si>
+    <t>MECSYCO</t>
+  </si>
+  <si>
+    <t>DACCOSIM</t>
+  </si>
+  <si>
+    <t>UMoC++</t>
+  </si>
+  <si>
+    <t>Lingua Franca</t>
+  </si>
+  <si>
+    <t>Reo</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>BIP (ADL or coordination framework?)</t>
+  </si>
+  <si>
+    <t>Manifold</t>
+  </si>
+  <si>
+    <t>ForSyDe</t>
+  </si>
+  <si>
+    <t>Coordination</t>
+  </si>
+  <si>
+    <t>Elements of coordination</t>
+  </si>
+  <si>
+    <t>Event-Scheduling</t>
+  </si>
+  <si>
+    <t>Event-Scheduling, Data-Exchange</t>
+  </si>
+  <si>
+    <t>Data-Exchange</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Data-Exchange ?</t>
+  </si>
+  <si>
+    <t>Data-Exchange, ?</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Dedicated elements</t>
+  </si>
+  <si>
+    <t>Query based</t>
+  </si>
+  <si>
+    <t>Architecture based</t>
+  </si>
+  <si>
+    <t>Architecture based ?</t>
+  </si>
+  <si>
+    <t>Name based</t>
+  </si>
+  <si>
+    <t>Architecture based?</t>
+  </si>
+  <si>
+    <t>Expressiveness</t>
+  </si>
+  <si>
+    <t>Predefined</t>
+  </si>
+  <si>
+    <t>Customizable</t>
+  </si>
+  <si>
+    <t>Predefined?</t>
+  </si>
+  <si>
+    <t>Model of Computation</t>
+  </si>
+  <si>
+    <t>Logical</t>
+  </si>
+  <si>
+    <t>Logical, Physical, Causal</t>
+  </si>
+  <si>
+    <t>Logical, Causal</t>
+  </si>
+  <si>
+    <t>Causal</t>
+  </si>
+  <si>
+    <t>Physical, Logical, Causal</t>
+  </si>
+  <si>
+    <t>Physical, Causal</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>Execution</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>Formal verification</t>
+  </si>
+  <si>
+    <t>Custom properties</t>
+  </si>
+  <si>
+    <t>Predefined properties</t>
+  </si>
+  <si>
+    <t>Model checking?, Runtime monitoring</t>
+  </si>
+  <si>
+    <t>Model checking?</t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Formal language</t>
+  </si>
+  <si>
+    <t>Programming language</t>
+  </si>
+  <si>
+    <t>Co-Simulation</t>
+  </si>
+  <si>
+    <t>Programing Language</t>
+  </si>
+  <si>
+    <t>Unified Execution</t>
+  </si>
+  <si>
+    <t>Component languages</t>
+  </si>
+  <si>
+    <t>Heterogeneous</t>
+  </si>
+  <si>
+    <t>Homogeneous</t>
+  </si>
+  <si>
+    <t>Heterogeneous? Unclear</t>
+  </si>
+  <si>
+    <t>Heterogeneous?</t>
+  </si>
+  <si>
+    <t>Coordination specification</t>
+  </si>
+  <si>
+    <t>Non-Intrusive</t>
+  </si>
+  <si>
+    <t>Intrusive</t>
+  </si>
+  <si>
+    <t>Intrusive?</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Discrete event</t>
+  </si>
+  <si>
+    <t>Hybrid</t>
+  </si>
+  <si>
+    <t>Hybrid?</t>
+  </si>
+  <si>
+    <t>Work order</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>More potential approaches</t>
+  </si>
+  <si>
+    <t>Coordination framework/Co-simulation</t>
+  </si>
+  <si>
+    <t>Ptolemy + Modhelix</t>
+  </si>
+  <si>
+    <t>Fully classified</t>
+  </si>
+  <si>
+    <t>Coordination language</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Coordination framework</t>
+  </si>
+  <si>
+    <t>BCOOL</t>
+  </si>
+  <si>
+    <t>Mostly classified</t>
+  </si>
+  <si>
+    <t>ADL</t>
+  </si>
+  <si>
+    <t>Darwin</t>
+  </si>
+  <si>
+    <t>ADLs are quite diverse? Other examples we should look at? MontiArc paper and overview paper</t>
+  </si>
   <si>
     <t>Tim</t>
-  </si>
-  <si>
-    <t>BCOoL</t>
-  </si>
-  <si>
-    <t>Ptolemy</t>
-  </si>
-  <si>
-    <t>Wright (ADL)</t>
-  </si>
-  <si>
-    <t>MontiArc (ADL)</t>
-  </si>
-  <si>
-    <t>CommUnity (ADL)</t>
-  </si>
-  <si>
-    <t>Metropolis</t>
-  </si>
-  <si>
-    <t>MECSYCO</t>
-  </si>
-  <si>
-    <t>DACCOSIM</t>
-  </si>
-  <si>
-    <t>UMoC++</t>
-  </si>
-  <si>
-    <t>Lingua Franca</t>
-  </si>
-  <si>
-    <t>Reo</t>
-  </si>
-  <si>
-    <t>Linda</t>
-  </si>
-  <si>
-    <t>BIP (ADL or coordination framework?)</t>
-  </si>
-  <si>
-    <t>Manifold</t>
-  </si>
-  <si>
-    <t>ForSyDe</t>
-  </si>
-  <si>
-    <t>Coordination</t>
-  </si>
-  <si>
-    <t>Elements of coordination</t>
-  </si>
-  <si>
-    <t>Event-Scheduling</t>
-  </si>
-  <si>
-    <t>Event-Scheduling, Data-Exchange</t>
-  </si>
-  <si>
-    <t>Data-Exchange</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Data-Exchange ?</t>
-  </si>
-  <si>
-    <t>Data-Exchange, ?</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>Dedicated elements</t>
-  </si>
-  <si>
-    <t>Query based</t>
-  </si>
-  <si>
-    <t>Architecture based</t>
-  </si>
-  <si>
-    <t>Architecture based ?</t>
-  </si>
-  <si>
-    <t>Name based</t>
-  </si>
-  <si>
-    <t>Architecture based?</t>
-  </si>
-  <si>
-    <t>Expressiveness</t>
-  </si>
-  <si>
-    <t>Predefined</t>
-  </si>
-  <si>
-    <t>Customizable</t>
-  </si>
-  <si>
-    <t>Predefined?</t>
-  </si>
-  <si>
-    <t>Model of Computation</t>
-  </si>
-  <si>
-    <t>Logical</t>
-  </si>
-  <si>
-    <t>Logical, Physical, Causal</t>
-  </si>
-  <si>
-    <t>Logical, Causal</t>
-  </si>
-  <si>
-    <t>Causal</t>
-  </si>
-  <si>
-    <t>Physical, Logical, Causal</t>
-  </si>
-  <si>
-    <t>Physical, Causal</t>
-  </si>
-  <si>
-    <t>Goal</t>
-  </si>
-  <si>
-    <t>Execution</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Simulation</t>
-  </si>
-  <si>
-    <t>Formal verification</t>
-  </si>
-  <si>
-    <t>Custom properties</t>
-  </si>
-  <si>
-    <t>Predefined properties</t>
-  </si>
-  <si>
-    <t>Model checking?, Runtime monitoring</t>
-  </si>
-  <si>
-    <t>Model checking?</t>
-  </si>
-  <si>
-    <t>Properties</t>
-  </si>
-  <si>
-    <t>Implementation</t>
-  </si>
-  <si>
-    <t>Formal language</t>
-  </si>
-  <si>
-    <t>Programming language</t>
-  </si>
-  <si>
-    <t>Co-Simulation</t>
-  </si>
-  <si>
-    <t>Programing Language</t>
-  </si>
-  <si>
-    <t>Unified Execution</t>
-  </si>
-  <si>
-    <t>Component languages</t>
-  </si>
-  <si>
-    <t>Heterogeneous</t>
-  </si>
-  <si>
-    <t>Homogeneous</t>
-  </si>
-  <si>
-    <t>Heterogeneous? Unclear</t>
-  </si>
-  <si>
-    <t>Heterogeneous?</t>
-  </si>
-  <si>
-    <t>Coordination specification</t>
-  </si>
-  <si>
-    <t>Non-Intrusive</t>
-  </si>
-  <si>
-    <t>Intrusive</t>
-  </si>
-  <si>
-    <t>Intrusive?</t>
-  </si>
-  <si>
-    <t>Domain</t>
-  </si>
-  <si>
-    <t>Discrete event</t>
-  </si>
-  <si>
-    <t>Hybrid</t>
-  </si>
-  <si>
-    <t>Hybrid?</t>
-  </si>
-  <si>
-    <t>Work order</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Approach</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Legend</t>
-  </si>
-  <si>
-    <t>More potential approaches</t>
-  </si>
-  <si>
-    <t>Coordination framework/Co-simulation</t>
-  </si>
-  <si>
-    <t>Ptolemy + Modhelix</t>
-  </si>
-  <si>
-    <t>Fully classified</t>
-  </si>
-  <si>
-    <t>Coordination language</t>
-  </si>
-  <si>
-    <t>Gamma</t>
-  </si>
-  <si>
-    <t>Coordination framework</t>
-  </si>
-  <si>
-    <t>BCOOL</t>
-  </si>
-  <si>
-    <t>Mostly classified</t>
-  </si>
-  <si>
-    <t>ADL</t>
-  </si>
-  <si>
-    <t>Darwin</t>
-  </si>
-  <si>
-    <t>ADLs are quite diverse? Other examples we should look at? MontiArc paper and overview paper</t>
   </si>
   <si>
     <t>Not classified</t>
@@ -1816,10 +1819,10 @@
         <v>82</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5">
@@ -1831,10 +1834,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6">
@@ -1846,7 +1849,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7">
@@ -1864,7 +1867,7 @@
         <v>80</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G8" s="14"/>
     </row>
@@ -1874,7 +1877,7 @@
         <v>85</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F9" s="14"/>
     </row>
@@ -1884,7 +1887,7 @@
         <v>85</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11">
@@ -1893,7 +1896,7 @@
         <v>85</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12">
@@ -1902,19 +1905,19 @@
         <v>80</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5"/>
       <c r="B13" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14">
@@ -1928,10 +1931,10 @@
         <v>15</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15">
@@ -1953,13 +1956,13 @@
         <v>21</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17">
@@ -1970,21 +1973,21 @@
         <v>21</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19">
@@ -1993,10 +1996,10 @@
         <v>85</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20">
@@ -2005,27 +2008,27 @@
         <v>85</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6"/>
       <c r="B21" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23">
@@ -2036,7 +2039,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24">
@@ -2044,25 +2047,25 @@
         <v>85</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change script readme and raw data
</commit_message>
<xml_diff>
--- a/artifacts/classification.xlsx
+++ b/artifacts/classification.xlsx
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="119">
   <si>
     <t>BCoordLang</t>
   </si>
@@ -233,13 +233,13 @@
     <t>Ptolemy</t>
   </si>
   <si>
-    <t>Wright (ADL)</t>
-  </si>
-  <si>
-    <t>MontiArc (ADL)</t>
-  </si>
-  <si>
-    <t>CommUnity (ADL)</t>
+    <t>Wright</t>
+  </si>
+  <si>
+    <t>MontiArc</t>
+  </si>
+  <si>
+    <t>CommUnity</t>
   </si>
   <si>
     <t>Metropolis</t>
@@ -263,7 +263,7 @@
     <t>Linda</t>
   </si>
   <si>
-    <t>BIP (ADL or coordination framework?)</t>
+    <t>BIP</t>
   </si>
   <si>
     <t>Manifold</t>
@@ -503,15 +503,6 @@
     <t>Linguage Franca</t>
   </si>
   <si>
-    <t>MontiArc</t>
-  </si>
-  <si>
-    <t>Wright</t>
-  </si>
-  <si>
-    <t>CommUnity</t>
-  </si>
-  <si>
     <t>REO</t>
   </si>
   <si>
@@ -555,6 +546,9 @@
   </si>
   <si>
     <t>Together with FMI</t>
+  </si>
+  <si>
+    <t>ADL or coordination framework?</t>
   </si>
   <si>
     <t>BIP?</t>
@@ -1003,15 +997,14 @@
     <col customWidth="1" min="3" max="3" width="15.38"/>
     <col customWidth="1" min="4" max="4" width="13.5"/>
     <col customWidth="1" min="5" max="5" width="25.63"/>
-    <col customWidth="1" min="6" max="6" width="18.63"/>
+    <col customWidth="1" min="6" max="6" width="16.25"/>
     <col customWidth="1" min="7" max="8" width="17.63"/>
     <col customWidth="1" min="9" max="9" width="28.25"/>
     <col customWidth="1" min="10" max="10" width="13.25"/>
     <col customWidth="1" min="11" max="11" width="12.13"/>
     <col customWidth="1" min="12" max="12" width="12.75"/>
     <col customWidth="1" min="13" max="13" width="19.38"/>
-    <col customWidth="1" min="14" max="15" width="18.13"/>
-    <col customWidth="1" min="16" max="16" width="31.13"/>
+    <col customWidth="1" min="14" max="16" width="18.13"/>
     <col customWidth="1" min="17" max="17" width="15.5"/>
     <col customWidth="1" min="18" max="18" width="13.63"/>
     <col customWidth="1" min="19" max="19" width="31.25"/>
@@ -1877,7 +1870,7 @@
         <v>85</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>93</v>
+        <v>4</v>
       </c>
       <c r="F9" s="14"/>
     </row>
@@ -1887,7 +1880,7 @@
         <v>85</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>94</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -1896,7 +1889,7 @@
         <v>85</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>95</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -1905,19 +1898,19 @@
         <v>80</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5"/>
       <c r="B13" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14">
@@ -1931,10 +1924,10 @@
         <v>15</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15">
@@ -1956,13 +1949,13 @@
         <v>21</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17">
@@ -1973,21 +1966,21 @@
         <v>21</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19">
@@ -1996,22 +1989,22 @@
         <v>85</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6"/>
       <c r="B20" s="7" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21">
@@ -2020,7 +2013,7 @@
         <v>91</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22">
@@ -2028,7 +2021,7 @@
         <v>91</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23">
@@ -2039,7 +2032,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24">
@@ -2047,25 +2040,25 @@
         <v>85</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update classification and plots due to feature model changes
</commit_message>
<xml_diff>
--- a/artifacts/classification.xlsx
+++ b/artifacts/classification.xlsx
@@ -127,6 +127,11 @@
         <t xml:space="preserve">They have rendezvous, broadcast and causality as operators to connect ports.</t>
       </text>
     </comment>
+    <comment authorId="0" ref="R6">
+      <text>
+        <t xml:space="preserve">Physical time is referred to in the continuous time MoC.</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="P8">
       <text>
         <t xml:space="preserve">Generates unified or distributed C/C++ programs.</t>
@@ -211,6 +216,18 @@
 Generates promela for formal verification</t>
       </text>
     </comment>
+    <comment authorId="0" ref="J12">
+      <text>
+        <t xml:space="preserve">SystemC and C++ for SImulation,
+Generates promela for formal verification</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="K12">
+      <text>
+        <t xml:space="preserve">SystemC and C++ for SImulation,
+Generates promela for formal verification</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="L12">
       <text>
         <t xml:space="preserve">Based on C++ templates</t>
@@ -338,6 +355,21 @@
     <comment authorId="0" ref="Q14">
       <text>
         <t xml:space="preserve">Components exchange data through ports similar to ADLs.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="K17">
+      <text>
+        <t xml:space="preserve">One step further it is even distributed.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="M17">
+      <text>
+        <t xml:space="preserve">They are working towards a distributed execution of the federation which is one step further like DACCOSIM.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="P17">
+      <text>
+        <t xml:space="preserve">Driven by an engine that used the generated code.</t>
       </text>
     </comment>
     <comment authorId="0" ref="J6">
@@ -351,7 +383,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="104">
   <si>
     <t>BCoorLang</t>
   </si>
@@ -491,112 +523,127 @@
     <t>Formal language</t>
   </si>
   <si>
-    <t>Programming language</t>
+    <t>General purpose language</t>
+  </si>
+  <si>
+    <t>Component languages</t>
+  </si>
+  <si>
+    <t>Heterogeneous</t>
+  </si>
+  <si>
+    <t>Homogeneous</t>
+  </si>
+  <si>
+    <t>Specification</t>
+  </si>
+  <si>
+    <t>Exogenous</t>
+  </si>
+  <si>
+    <t>Endogenous</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Discrete event</t>
+  </si>
+  <si>
+    <t>Hybrid</t>
+  </si>
+  <si>
+    <t>Component transparency</t>
+  </si>
+  <si>
+    <t>White-box</t>
+  </si>
+  <si>
+    <t>Black-box</t>
+  </si>
+  <si>
+    <t>Centralized</t>
+  </si>
+  <si>
+    <t>Federated</t>
+  </si>
+  <si>
+    <t>Coordination language</t>
+  </si>
+  <si>
+    <t>Coordination framework</t>
+  </si>
+  <si>
+    <t>Co-simulation approach</t>
+  </si>
+  <si>
+    <t>Architecture description language</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>Color code</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>More potential approaches</t>
+  </si>
+  <si>
+    <t>Fully classified</t>
+  </si>
+  <si>
+    <t>Coordination framework/Co-simulation</t>
+  </si>
+  <si>
+    <t>Ptolemy + Modhelix</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Mostly classified</t>
+  </si>
+  <si>
+    <t>BCOOL</t>
+  </si>
+  <si>
+    <t>ADL</t>
+  </si>
+  <si>
+    <t>Darwin</t>
+  </si>
+  <si>
+    <t>OG ADL like Wright</t>
+  </si>
+  <si>
+    <t>Not classified</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Gama</t>
+  </si>
+  <si>
+    <t>https://gama-platform.org/wiki/MultiParadigmModeling</t>
+  </si>
+  <si>
+    <t>No coordination</t>
   </si>
   <si>
     <t>Co-Simulation</t>
-  </si>
-  <si>
-    <t>Component languages</t>
-  </si>
-  <si>
-    <t>Heterogeneous</t>
-  </si>
-  <si>
-    <t>Homogeneous</t>
-  </si>
-  <si>
-    <t>Specification</t>
-  </si>
-  <si>
-    <t>Exogenous</t>
-  </si>
-  <si>
-    <t>Endogenous</t>
-  </si>
-  <si>
-    <t>Domain</t>
-  </si>
-  <si>
-    <t>Discrete event</t>
-  </si>
-  <si>
-    <t>Hybrid</t>
-  </si>
-  <si>
-    <t>Coordination language</t>
-  </si>
-  <si>
-    <t>Coordination framework</t>
-  </si>
-  <si>
-    <t>Co-simulation tool</t>
-  </si>
-  <si>
-    <t>Architecture description language</t>
-  </si>
-  <si>
-    <t>Misc</t>
-  </si>
-  <si>
-    <t>Color code</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Approach</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>More potential approaches</t>
-  </si>
-  <si>
-    <t>Fully classified</t>
-  </si>
-  <si>
-    <t>Coordination framework/Co-simulation</t>
-  </si>
-  <si>
-    <t>Ptolemy + Modhelix</t>
-  </si>
-  <si>
-    <t>Gamma</t>
-  </si>
-  <si>
-    <t>Mostly classified</t>
-  </si>
-  <si>
-    <t>BCOOL</t>
-  </si>
-  <si>
-    <t>ADL</t>
-  </si>
-  <si>
-    <t>Darwin</t>
-  </si>
-  <si>
-    <t>OG ADL like Wright</t>
-  </si>
-  <si>
-    <t>Not classified</t>
-  </si>
-  <si>
-    <t>Tim</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Gama</t>
-  </si>
-  <si>
-    <t>https://gama-platform.org/wiki/MultiParadigmModeling</t>
-  </si>
-  <si>
-    <t>No coordination</t>
   </si>
   <si>
     <t>Symthesis</t>
@@ -1090,16 +1137,13 @@
     <col customWidth="1" min="2" max="2" width="21.75"/>
     <col customWidth="1" min="3" max="3" width="15.38"/>
     <col customWidth="1" min="4" max="4" width="19.5"/>
-    <col customWidth="1" min="5" max="5" width="26.75"/>
+    <col customWidth="1" min="5" max="5" width="25.63"/>
     <col customWidth="1" min="6" max="6" width="16.25"/>
-    <col customWidth="1" min="7" max="9" width="17.63"/>
-    <col customWidth="1" min="10" max="11" width="14.63"/>
-    <col customWidth="1" min="12" max="12" width="18.13"/>
-    <col customWidth="1" min="13" max="13" width="19.38"/>
+    <col customWidth="1" min="7" max="13" width="19.88"/>
     <col customWidth="1" min="14" max="14" width="25.63"/>
-    <col customWidth="1" min="15" max="15" width="18.13"/>
+    <col customWidth="1" min="15" max="15" width="19.88"/>
     <col customWidth="1" min="16" max="16" width="25.63"/>
-    <col customWidth="1" min="17" max="17" width="17.63"/>
+    <col customWidth="1" min="17" max="17" width="19.88"/>
     <col customWidth="1" min="18" max="18" width="25.63"/>
     <col customWidth="1" min="19" max="19" width="31.25"/>
     <col customWidth="1" min="20" max="20" width="30.0"/>
@@ -1383,7 +1427,7 @@
         <v>35</v>
       </c>
       <c r="R6" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
@@ -1548,10 +1592,10 @@
         <v>46</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>46</v>
@@ -1577,181 +1621,279 @@
     </row>
     <row r="13">
       <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="I13" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="L13" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N13" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P13" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q13" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R13" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="H14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="M14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="N14" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="O14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="P14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="R14" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="L14" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="N14" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="O14" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="P14" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q14" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="R14" s="10" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="F15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="K15" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="R15" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="N15" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="O15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="P15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="R15" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="16" t="s">
+      <c r="C16" s="10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="17" t="s">
+      <c r="D16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="10" t="s">
         <v>58</v>
       </c>
+      <c r="K16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="R16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="S16" s="11"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="P17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="R17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="S17" s="11"/>
     </row>
     <row r="20">
-      <c r="A20" s="18" t="s">
-        <v>59</v>
+      <c r="A20" s="16" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="19" t="s">
-        <v>60</v>
+      <c r="A21" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -1766,11 +1908,14 @@
       <c r="R21" s="11"/>
     </row>
     <row r="22">
-      <c r="A22" s="20" t="s">
-        <v>61</v>
+      <c r="A22" s="18" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="23">
+      <c r="A23" s="19" t="s">
+        <v>64</v>
+      </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -1783,6 +1928,11 @@
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
       <c r="R23" s="11"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="20" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="43">
       <c r="D43" s="11"/>
@@ -1842,148 +1992,148 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="21" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="25" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="24" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="27" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="11"/>
       <c r="B6" s="23" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="11"/>
       <c r="B7" s="23" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="11"/>
       <c r="B8" s="23" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="G8" s="12"/>
     </row>
     <row r="9">
       <c r="A9" s="10"/>
       <c r="B9" s="23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>4</v>
@@ -1993,7 +2143,7 @@
     <row r="10">
       <c r="A10" s="10"/>
       <c r="B10" s="23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>3</v>
@@ -2002,7 +2152,7 @@
     <row r="11">
       <c r="A11" s="10"/>
       <c r="B11" s="23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>5</v>
@@ -2011,31 +2161,31 @@
     <row r="12">
       <c r="A12" s="10"/>
       <c r="B12" s="23" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="10"/>
       <c r="B13" s="23" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="10"/>
       <c r="B14" s="23" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C14" s="28" t="s">
         <v>15</v>
@@ -2044,7 +2194,7 @@
     <row r="15">
       <c r="A15" s="10"/>
       <c r="B15" s="23" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>6</v>
@@ -2052,19 +2202,19 @@
     </row>
     <row r="16">
       <c r="B16" s="23" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="10"/>
       <c r="B17" s="23" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>13</v>
@@ -2073,7 +2223,7 @@
     <row r="18">
       <c r="A18" s="11"/>
       <c r="B18" s="23" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C18" s="29" t="s">
         <v>9</v>
@@ -2081,18 +2231,18 @@
     </row>
     <row r="19">
       <c r="B19" s="23" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="23" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>